<commit_message>
transfer to py scripts done
</commit_message>
<xml_diff>
--- a/input/concentrations/ds.3p.2eq/xlsx/data.xlsx
+++ b/input/concentrations/ds.3p.2eq/xlsx/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\wannabecoder\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEVreplica\input\concentrations\ds.3p.2eq\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="11475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="11475" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -873,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -997,9 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>